<commit_message>
subindo atualizacao de planilha com spl para astro-ph
</commit_message>
<xml_diff>
--- a/PredLig/src/Documentation/Execution of 1994-1999.xlsx
+++ b/PredLig/src/Documentation/Execution of 1994-1999.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14620" tabRatio="988" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20700" windowHeight="11760" tabRatio="988" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1994-1999" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="81">
   <si>
     <t>DataSet</t>
   </si>
@@ -270,13 +270,16 @@
   </si>
   <si>
     <t>DJC</t>
+  </si>
+  <si>
+    <t>SPL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -511,22 +514,22 @@
     </xf>
   </cellXfs>
   <cellStyles count="16">
-    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -637,7 +640,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -707,13 +710,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4.668011738811445</c:v>
+                  <c:v>4.6680117388114448</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.364949130292091</c:v>
+                  <c:v>4.3649491302920911</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.275030366128752</c:v>
+                  <c:v>5.2750303661287523</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -771,13 +774,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4.897285399853265</c:v>
+                  <c:v>4.8972853998532653</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.511650804069576</c:v>
+                  <c:v>3.5116508040695762</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.4070796460177</c:v>
+                  <c:v>8.4070796460176993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -838,10 +841,10 @@
                   <c:v>5.30997798972854</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.463406629471612</c:v>
+                  <c:v>4.4634066294716117</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.081901787263578</c:v>
+                  <c:v>6.0819017872635781</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -905,7 +908,7 @@
                   <c:v>3.413193304890056</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.30938747180288</c:v>
+                  <c:v>9.3093874718028804</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -963,13 +966,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4.356199559794571</c:v>
+                  <c:v>4.3561995597945709</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.855267476206104</c:v>
+                  <c:v>2.8552674762061043</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.719416970327955</c:v>
+                  <c:v>8.7194169703279556</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1027,13 +1030,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5.282465150403521</c:v>
+                  <c:v>5.2824651504035218</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.642927469642271</c:v>
+                  <c:v>3.6429274696422711</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.979698073919834</c:v>
+                  <c:v>8.9796980739198347</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1091,13 +1094,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3.356566397652238</c:v>
+                  <c:v>3.3565663976522377</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.673777486051854</c:v>
+                  <c:v>1.6737774860518542</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.322748568453931</c:v>
+                  <c:v>5.3227485684539309</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1155,13 +1158,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.504402054292003</c:v>
+                  <c:v>0.50440205429200291</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.426649163111257</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.741801145236856</c:v>
+                  <c:v>0.74180114523685581</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1219,13 +1222,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4.91562729273661</c:v>
+                  <c:v>4.9156272927366098</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.758779127010173</c:v>
+                  <c:v>4.7587791270101736</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.431025507548152</c:v>
+                  <c:v>7.4310255075481519</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1283,13 +1286,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4.594644167278063</c:v>
+                  <c:v>4.5946441672780631</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.102395799146702</c:v>
+                  <c:v>4.1023957991467022</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.634912372028458</c:v>
+                  <c:v>7.6349123720284577</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1347,13 +1350,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4.91562729273661</c:v>
+                  <c:v>4.9156272927366098</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.839842468001313</c:v>
+                  <c:v>3.8398424680013128</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.595870206489676</c:v>
+                  <c:v>7.5958702064896757</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1411,13 +1414,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5.218268525311811</c:v>
+                  <c:v>5.218268525311812</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.08500164095832</c:v>
+                  <c:v>3.0850016409583199</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.50043380183932</c:v>
+                  <c:v>7.5004338018393195</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1432,11 +1435,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2109233976"/>
-        <c:axId val="2109237192"/>
+        <c:axId val="42055168"/>
+        <c:axId val="34282816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2109233976"/>
+        <c:axId val="42055168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1445,7 +1448,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109237192"/>
+        <c:crossAx val="34282816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1453,7 +1456,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2109237192"/>
+        <c:axId val="34282816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1464,7 +1467,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109233976"/>
+        <c:crossAx val="42055168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1480,7 +1483,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.787401575" l="0.511811024" r="0.511811024" t="0.787401575" header="0.31496062" footer="0.31496062"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1489,7 +1492,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pt-BR"/>
   <c:roundedCorners val="1"/>
   <c:style val="2"/>
   <c:chart>
@@ -1598,7 +1601,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>133.0</c:v>
+                  <c:v>133</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1666,7 +1669,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>123.0</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1734,7 +1737,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>121.0</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1802,7 +1805,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>19.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1870,7 +1873,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>125.0</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1938,7 +1941,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>126.0</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2006,7 +2009,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>133.0</c:v>
+                  <c:v>133</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2036,12 +2039,12 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="2110261960"/>
-        <c:axId val="2110265192"/>
+        <c:axId val="518296576"/>
+        <c:axId val="43156032"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="2110261960"/>
+        <c:axId val="518296576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2058,7 +2061,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2110265192"/>
+        <c:crossAx val="43156032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2066,7 +2069,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2110265192"/>
+        <c:axId val="43156032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2092,7 +2095,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2110261960"/>
+        <c:crossAx val="518296576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2129,7 +2132,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.787401575" l="0.511811024" r="0.511811024" t="0.787401575" header="0.31496062" footer="0.31496062"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2498,13 +2501,13 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" customWidth="1"/>
-    <col min="6" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2523,7 +2526,7 @@
       <c r="G3" s="18"/>
       <c r="H3" s="19"/>
     </row>
-    <row r="4" spans="2:8" ht="22.75" customHeight="1">
+    <row r="4" spans="2:8" ht="22.7" customHeight="1">
       <c r="B4" s="16"/>
       <c r="C4" s="1" t="s">
         <v>1</v>
@@ -2544,7 +2547,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="22.75" customHeight="1" thickTop="1" thickBot="1">
+    <row r="5" spans="2:8" ht="22.7" customHeight="1" thickTop="1" thickBot="1">
       <c r="B5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2567,7 +2570,7 @@
         <v>10904</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="19.75" customHeight="1" thickTop="1" thickBot="1">
+    <row r="6" spans="2:8" ht="19.7" customHeight="1" thickTop="1" thickBot="1">
       <c r="B6" s="1" t="s">
         <v>74</v>
       </c>
@@ -2590,7 +2593,7 @@
         <v>3047</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="17" thickTop="1" thickBot="1">
+    <row r="7" spans="2:8" ht="16.5" thickTop="1" thickBot="1">
       <c r="B7" s="15" t="s">
         <v>75</v>
       </c>
@@ -2613,7 +2616,7 @@
         <v>23052</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="13" thickTop="1"/>
+    <row r="8" spans="2:8" ht="13.5" thickTop="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B3:B4"/>
@@ -2637,14 +2640,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C6:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+    <sheetView tabSelected="1" topLeftCell="G9" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="3:9">
@@ -2998,9 +3001,16 @@
       </c>
     </row>
     <row r="20" spans="3:9">
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
+      <c r="C20" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="13">
+        <f>(E20/'1994-1999'!H5)*100</f>
+        <v>3.163976522377109</v>
+      </c>
+      <c r="E20" s="13">
+        <v>345</v>
+      </c>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
@@ -3193,9 +3203,9 @@
       <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="2" max="2" width="8.83203125" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:22">
@@ -3405,7 +3415,7 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15">
       <c r="A1" s="9" t="s">
@@ -3512,7 +3522,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15">
       <c r="A1" s="9" t="s">
@@ -3627,7 +3637,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15">
       <c r="A1" s="9" t="s">
@@ -3742,7 +3752,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15">
       <c r="A1" s="9" t="s">
@@ -3859,7 +3869,7 @@
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15">
       <c r="A1" s="9" t="s">
@@ -3976,7 +3986,7 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15">
       <c r="A1" s="9" t="s">

</xml_diff>